<commit_message>
atualização de página principal e de cronograma da disciplina
</commit_message>
<xml_diff>
--- a/Planejamento_v02.xlsx
+++ b/Planejamento_v02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c67fd77eff8119b6/Ensino/Projeto e Tecnologia na Indústria da construção/projetoetecnologiaccv.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0AC1E8D-E3ED-1B42-9959-45C432E83248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A0AC1E8D-E3ED-1B42-9959-45C432E83248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95FB7AA0-590B-6547-AC64-584CD912D192}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Projeto e Tecnologia na industria da Construção</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Arquitetura contemporânea e automação (capítulo 1)</t>
   </si>
   <si>
-    <t>Tecnologias avançadas e a construção</t>
-  </si>
-  <si>
     <t>O que será abordado</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Tema de acordo com a demanda dos trabalhos que estão sendo desenvolvidos</t>
+  </si>
+  <si>
+    <t>Orientação e desenvolvimento de trabalhos</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -467,13 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -486,9 +480,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -813,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31600A02-DF54-1E42-8CA0-C9EF22301E91}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="181" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="A1:D23"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="181" zoomScaleSheetLayoutView="141" workbookViewId="0">
+      <selection sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -830,12 +821,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -849,10 +840,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>10</v>
@@ -894,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>19</v>
@@ -911,10 +902,10 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -928,23 +919,22 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="7">
         <v>44816</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="18"/>
+      <c r="C9" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
@@ -957,22 +947,19 @@
         <v>44823</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>8</v>
       </c>
       <c r="B11" s="7">
         <v>44830</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
+      <c r="C11" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -983,10 +970,10 @@
         <v>44837</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
@@ -1000,10 +987,10 @@
         <v>44844</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>19</v>
@@ -1017,27 +1004,27 @@
         <v>44851</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
+    <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>12</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="7">
         <v>44858</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>31</v>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1048,7 +1035,7 @@
         <v>44865</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="10"/>
     </row>
@@ -1060,10 +1047,10 @@
         <v>44872</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1074,10 +1061,10 @@
         <v>44879</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1088,10 +1075,10 @@
         <v>44886</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -1102,10 +1089,10 @@
         <v>44893</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1116,28 +1103,28 @@
         <v>44900</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="14">
+      <c r="B22" s="12">
         <v>44907</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="20"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14">
         <v>44914</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>